<commit_message>
update result 20200911 / plan 20200912
</commit_message>
<xml_diff>
--- a/20200911.xlsx
+++ b/20200911.xlsx
@@ -1,38 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Polaris Office Sheet" lastEdited="7" lowestEdited="7" rupBuild="8.1.852.35783"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA10AF3-F442-4056-B9F4-36266CA0F56A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1365" windowWidth="27000" windowHeight="14235" tabRatio="580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="570" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>수행</t>
   </si>
@@ -203,186 +188,207 @@
   </si>
   <si>
     <t xml:space="preserve">잤다 </t>
-    <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
     <t>잠안와서 3시30분에 잠듬</t>
-    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행하긴 하였으나, 로컬모드</t>
+  </si>
+  <si>
+    <t>진행하긴 하였으나, 로컬모드
+마무리는 하지 못함</t>
+  </si>
+  <si>
+    <t>진행하긴 하였으나, 로컬모드
+마무리는 하지 못함, UI또한 마무리 못함</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="22" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="64" formatCode="&quot;₩&quot;#,##0;\\\-&quot;₩&quot;#,##0"/>
+  </numFmts>
+  <fonts count="30">
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-    </font>
-    <font>
-      <sz val="11"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF0563C1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF954F72"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <sz val="18.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF44546A"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF44546A"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF44546A"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF44546A"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF3F3F76"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF3F3F3F"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF006100"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF9C0006"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF9C6500"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF7F7F7F"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <name val="돋움"/>
+      <color rgb="FF000000"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="10"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color rgb="FF954F72"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF44546A"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="11"/>
+    </font>
+    <font>
+      <sz val="18.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color rgb="FF44546A"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <sz val="15.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color rgb="FF44546A"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <sz val="13.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF44546A"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFFFFFF"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="돋움"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="0"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="1"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="62">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -567,23 +573,185 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF36B700"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF009900"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -728,16 +896,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -756,23 +924,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
@@ -780,14 +948,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -816,7 +984,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -829,7 +997,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
@@ -840,7 +1008,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -848,48 +1016,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.399980"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
@@ -901,100 +1203,232 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="26" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="27" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="26" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="28" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="37" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="38" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="39" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="40" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="41" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="42" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="43" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="44" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="45" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="46" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="47" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="48" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="49" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="50" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="51" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="52" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="53" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="54" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="55" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="56" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="57" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="58" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1035,79 +1469,61 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="20" fontId="0" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1119,55 +1535,136 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="60" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="60" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="60" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="60" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="44">
-    <cellStyle name="20% - 강조색1" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - 강조색2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - 강조색3" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - 강조색4" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - 강조색5" xfId="10" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - 강조색6" xfId="12" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - 강조색1" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - 강조색2" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - 강조색3" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - 강조색4" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - 강조색5" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - 강조색6" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - 강조색1" xfId="32" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - 강조색2" xfId="34" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - 강조색3" xfId="36" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - 강조색4" xfId="38" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - 강조색5" xfId="40" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - 강조색6" xfId="42" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="강조색1" xfId="31" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="강조색2" xfId="33" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="강조색3" xfId="35" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="강조색4" xfId="37" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="강조색5" xfId="39" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="강조색6" xfId="41" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="경고문" xfId="16" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="계산" xfId="24" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="나쁨" xfId="29" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="메모" xfId="1" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="보통" xfId="30" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="설명텍스트" xfId="43" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="셀 확인" xfId="25" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="연결된 셀" xfId="26" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="열어본 하이퍼링크" xfId="15" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="요약" xfId="27" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="입력" xfId="22" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="제목" xfId="17" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="제목 1" xfId="18" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="제목 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="제목 3" xfId="20" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="제목 4" xfId="21" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="좋음" xfId="28" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="출력" xfId="23" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+  <cellStyles count="92">
+    <cellStyle name="20% - 강조색1" xfId="68" builtinId="30"/>
+    <cellStyle name="20% - 강조색2" xfId="72" builtinId="34"/>
+    <cellStyle name="20% - 강조색3" xfId="76" builtinId="38"/>
+    <cellStyle name="20% - 강조색4" xfId="80" builtinId="42"/>
+    <cellStyle name="20% - 강조색5" xfId="84" builtinId="46"/>
+    <cellStyle name="20% - 강조색6" xfId="88" builtinId="50"/>
+    <cellStyle name="40% - 강조색1" xfId="69" builtinId="31"/>
+    <cellStyle name="40% - 강조색2" xfId="73" builtinId="35"/>
+    <cellStyle name="40% - 강조색3" xfId="77" builtinId="39"/>
+    <cellStyle name="40% - 강조색4" xfId="81" builtinId="43"/>
+    <cellStyle name="40% - 강조색5" xfId="85" builtinId="47"/>
+    <cellStyle name="40% - 강조색6" xfId="89" builtinId="51"/>
+    <cellStyle name="60% - 강조색1" xfId="70" builtinId="32"/>
+    <cellStyle name="60% - 강조색2" xfId="74" builtinId="36"/>
+    <cellStyle name="60% - 강조색3" xfId="78" builtinId="40"/>
+    <cellStyle name="60% - 강조색4" xfId="82" builtinId="44"/>
+    <cellStyle name="60% - 강조색5" xfId="86" builtinId="48"/>
+    <cellStyle name="60% - 강조색6" xfId="90" builtinId="52"/>
+    <cellStyle name="강조색1" xfId="67" builtinId="29"/>
+    <cellStyle name="강조색2" xfId="71" builtinId="33"/>
+    <cellStyle name="강조색3" xfId="75" builtinId="37"/>
+    <cellStyle name="강조색4" xfId="79" builtinId="41"/>
+    <cellStyle name="강조색5" xfId="83" builtinId="45"/>
+    <cellStyle name="강조색6" xfId="87" builtinId="49"/>
+    <cellStyle name="경고문" xfId="52" builtinId="11"/>
+    <cellStyle name="계산" xfId="60" builtinId="22"/>
+    <cellStyle name="나쁨" xfId="65" builtinId="27"/>
+    <cellStyle name="메모" xfId="51" builtinId="10"/>
+    <cellStyle name="백분율" xfId="46" builtinId="5"/>
+    <cellStyle name="보통" xfId="66" builtinId="28"/>
+    <cellStyle name="설명텍스트" xfId="91" builtinId="53"/>
+    <cellStyle name="셀 확인" xfId="61" builtinId="23"/>
+    <cellStyle name="쉼표" xfId="44" builtinId="3"/>
+    <cellStyle name="쉼표[0]" xfId="47" builtinId="6"/>
+    <cellStyle name="연결된 셀" xfId="62" builtinId="24"/>
+    <cellStyle name="열어본 하이퍼링크" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="요약" xfId="63" builtinId="25"/>
+    <cellStyle name="입력" xfId="58" builtinId="20"/>
+    <cellStyle name="제목" xfId="53" builtinId="15"/>
+    <cellStyle name="제목 1" xfId="54" builtinId="16"/>
+    <cellStyle name="제목 2" xfId="55" builtinId="17"/>
+    <cellStyle name="제목 3" xfId="56" builtinId="18"/>
+    <cellStyle name="제목 4" xfId="57" builtinId="19"/>
+    <cellStyle name="좋음" xfId="64" builtinId="26"/>
+    <cellStyle name="출력" xfId="59" builtinId="21"/>
+    <cellStyle name="통화" xfId="45" builtinId="4"/>
+    <cellStyle name="통화[0]" xfId="48" builtinId="7"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="14" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="하이퍼링크" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="20% - 강조색1" xfId="2"/>
+    <cellStyle name="20% - 강조색2" xfId="4"/>
+    <cellStyle name="20% - 강조색3" xfId="6"/>
+    <cellStyle name="20% - 강조색4" xfId="8"/>
+    <cellStyle name="20% - 강조색5" xfId="10"/>
+    <cellStyle name="20% - 강조색6" xfId="12"/>
+    <cellStyle name="40% - 강조색1" xfId="3"/>
+    <cellStyle name="40% - 강조색2" xfId="5"/>
+    <cellStyle name="40% - 강조색3" xfId="7"/>
+    <cellStyle name="40% - 강조색4" xfId="9"/>
+    <cellStyle name="40% - 강조색5" xfId="11"/>
+    <cellStyle name="40% - 강조색6" xfId="13"/>
+    <cellStyle name="60% - 강조색1" xfId="32"/>
+    <cellStyle name="60% - 강조색2" xfId="34"/>
+    <cellStyle name="60% - 강조색3" xfId="36"/>
+    <cellStyle name="60% - 강조색4" xfId="38"/>
+    <cellStyle name="60% - 강조색5" xfId="40"/>
+    <cellStyle name="60% - 강조색6" xfId="42"/>
+    <cellStyle name="강조색1" xfId="31"/>
+    <cellStyle name="강조색2" xfId="33"/>
+    <cellStyle name="강조색3" xfId="35"/>
+    <cellStyle name="강조색4" xfId="37"/>
+    <cellStyle name="강조색5" xfId="39"/>
+    <cellStyle name="강조색6" xfId="41"/>
+    <cellStyle name="경고문" xfId="16"/>
+    <cellStyle name="계산" xfId="24"/>
+    <cellStyle name="나쁨" xfId="29"/>
+    <cellStyle name="메모" xfId="1"/>
+    <cellStyle name="보통" xfId="30"/>
+    <cellStyle name="설명텍스트" xfId="43"/>
+    <cellStyle name="셀 확인" xfId="25"/>
+    <cellStyle name="연결된 셀" xfId="26"/>
+    <cellStyle name="열어본 하이퍼링크" xfId="15"/>
+    <cellStyle name="요약" xfId="27"/>
+    <cellStyle name="입력" xfId="22"/>
+    <cellStyle name="제목" xfId="17"/>
+    <cellStyle name="제목 1" xfId="18"/>
+    <cellStyle name="제목 2" xfId="19"/>
+    <cellStyle name="제목 3" xfId="20"/>
+    <cellStyle name="제목 4" xfId="21"/>
+    <cellStyle name="좋음" xfId="28"/>
+    <cellStyle name="출력" xfId="23"/>
+    <cellStyle name="하이퍼링크" xfId="14"/>
   </cellStyles>
   <dxfs count="16">
     <dxf>
@@ -1200,11 +1697,14 @@
         <right style="thin">
           <color rgb="FFBFBFBF"/>
         </right>
+        <diagonal/>
       </border>
     </dxf>
     <dxf>
       <font>
         <b/>
+        <sz val="11.0"/>
+        <name val="맑은 고딕"/>
         <color rgb="FF000000"/>
       </font>
       <border>
@@ -1214,11 +1714,14 @@
         <bottom style="thin">
           <color rgb="FF5B9BD5"/>
         </bottom>
+        <diagonal/>
       </border>
     </dxf>
     <dxf>
       <font>
         <b/>
+        <sz val="11.0"/>
+        <name val="맑은 고딕"/>
         <color rgb="FF000000"/>
       </font>
       <border>
@@ -1228,23 +1731,29 @@
         <bottom style="thin">
           <color rgb="FF5B9BD5"/>
         </bottom>
+        <diagonal/>
       </border>
     </dxf>
     <dxf>
       <font>
         <b/>
+        <sz val="11.0"/>
+        <name val="맑은 고딕"/>
         <color rgb="FF000000"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
+        <sz val="11.0"/>
+        <name val="맑은 고딕"/>
         <color rgb="FF000000"/>
       </font>
       <border>
         <bottom style="thin">
           <color rgb="FF9CC3E6"/>
         </bottom>
+        <diagonal/>
       </border>
     </dxf>
     <dxf>
@@ -1277,6 +1786,7 @@
         <bottom style="thin">
           <color rgb="FF315F97"/>
         </bottom>
+        <diagonal/>
       </border>
     </dxf>
     <dxf>
@@ -1301,6 +1811,7 @@
         <bottom style="thin">
           <color rgb="FF315F97"/>
         </bottom>
+        <diagonal/>
       </border>
     </dxf>
     <dxf>
@@ -1322,6 +1833,8 @@
     <dxf>
       <font>
         <b/>
+        <sz val="11.0"/>
+        <name val="맑은 고딕"/>
         <color rgb="FF000000"/>
       </font>
       <fill>
@@ -1334,11 +1847,14 @@
         <bottom style="thin">
           <color rgb="FF9CC3E6"/>
         </bottom>
+        <diagonal/>
       </border>
     </dxf>
     <dxf>
       <font>
         <b/>
+        <sz val="11.0"/>
+        <name val="맑은 고딕"/>
         <color rgb="FF000000"/>
       </font>
       <fill>
@@ -1351,11 +1867,12 @@
         <top style="thin">
           <color rgb="FF9CC3E6"/>
         </top>
+        <diagonal/>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Normal Style 1 - Accent 1" pivot="0" count="8" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Normal Style 1 - Accent 1" pivot="0" count="8">
       <tableStyleElement type="headerRow" dxfId="15"/>
       <tableStyleElement type="totalRow" dxfId="14"/>
       <tableStyleElement type="firstColumn" dxfId="13"/>
@@ -1365,7 +1882,7 @@
       <tableStyleElement type="firstColumnStripe" dxfId="9"/>
       <tableStyleElement type="secondColumnStripe" dxfId="8"/>
     </tableStyle>
-    <tableStyle name="Light Style 1 - Accent 1" table="0" count="8" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Light Style 1 - Accent 1" pivot="1" count="8">
       <tableStyleElement type="wholeTable" dxfId="7"/>
       <tableStyleElement type="headerRow" dxfId="6"/>
       <tableStyleElement type="totalRow" dxfId="5"/>
@@ -1376,14 +1893,6 @@
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1644,380 +2153,383 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.87500000" defaultRowHeight="16.500000"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="42.75" customWidth="1"/>
-    <col min="6" max="6" width="25.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.75" customWidth="1"/>
-    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="78" customWidth="1"/>
+    <col min="2" max="2" width="16.50500011" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="42.75500107" customWidth="1" outlineLevel="0"/>
+    <col min="6" max="6" width="25.12999916" customWidth="1" outlineLevel="0"/>
+    <col min="8" max="8" width="39.75500107" customWidth="1" outlineLevel="0"/>
+    <col min="10" max="10" width="9.88000011" customWidth="1" outlineLevel="0"/>
+    <col min="11" max="11" width="78.00499725" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:12">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
+    <row r="3" spans="2:12">
+      <c r="B3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="45" t="s">
+      <c r="E3" s="33"/>
+      <c r="F3" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>36</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="30"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="36"/>
-      <c r="H4" t="s">
+    <row r="4" spans="2:12">
+      <c r="B4" s="6"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="28"/>
+      <c r="H4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="36"/>
-      <c r="H5" t="s">
+    <row r="5" spans="2:12">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="28"/>
+      <c r="H5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="30"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="36"/>
-      <c r="H6" t="s">
+    <row r="6" spans="2:12">
+      <c r="B6" s="6"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="28"/>
+      <c r="H6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="36"/>
-      <c r="H7" t="s">
+    <row r="7" spans="2:12">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="28"/>
+      <c r="H7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <f>SUM(I3:I6)</f>
         <v>206</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="30"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="37"/>
-      <c r="H8" t="s">
+    <row r="8" spans="2:12">
+      <c r="B8" s="6"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="29"/>
+      <c r="H8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:12" ht="16.300000" customHeight="1">
+      <c r="B9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="41" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="0">
         <v>309</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:12">
+      <c r="B10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="44" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="11" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+    <row r="11" spans="2:12" ht="16.300000" customHeight="1">
+      <c r="B11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="40"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="45"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="2:12">
+      <c r="B12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="17"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="46"/>
     </row>
-    <row r="13" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="2:12" ht="16.300000" customHeight="1">
+      <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="18"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="45"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="2:12">
+      <c r="B14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="18"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="45"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="2:12">
+      <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="18"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="45"/>
     </row>
-    <row r="16" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+    <row r="16" spans="2:12" ht="16.300000" customHeight="1">
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="28"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="45"/>
     </row>
-    <row r="17" spans="2:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="2:6" ht="16.300000" customHeight="1">
+      <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="28"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="45"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+    <row r="18" spans="2:6">
+      <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="18"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="47"/>
     </row>
-    <row r="19" spans="2:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
+    <row r="19" spans="2:6" ht="16.300000" customHeight="1">
+      <c r="B19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="18"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
+    <row r="20" spans="2:6">
+      <c r="B20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="18"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="15"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
+    <row r="21" spans="2:6">
+      <c r="B21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="18"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="15"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="9" t="s">
+    <row r="22" spans="2:6">
+      <c r="B22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="19"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="16"/>
     </row>
-    <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="2:6" ht="15.750000" customHeight="1">
+      <c r="B23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="20"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="24" spans="2:6">
+      <c r="B24" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="0" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="D19:D23"/>
-    <mergeCell ref="F16:F17"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="D3:D10"/>
-    <mergeCell ref="D11:D18"/>
     <mergeCell ref="E3:E8"/>
     <mergeCell ref="F3:F8"/>
+    <mergeCell ref="F10:F18"/>
+    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="D19:D23"/>
   </mergeCells>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.87500000" defaultRowHeight="16.500000"/>
   <sheetData/>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr codeName="Sheet3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.87500000" defaultRowHeight="16.500000"/>
   <sheetData/>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>